<commit_message>
started the form input part
</commit_message>
<xml_diff>
--- a/data/coffee-flavors_lexicon.xlsx
+++ b/data/coffee-flavors_lexicon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\W_shortcut\coffee_roasting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD42EA4A-6F5D-44A1-B80C-AB1848EB8F82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F0B861-4630-4DD0-A8DE-6CADB0019C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coffee-flavors_lexicon" sheetId="2" r:id="rId1"/>
@@ -1567,19 +1567,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>230</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>218</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>217</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>216</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>228</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -3769,17 +3769,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="A20:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3790,77 +3790,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>112</v>
       </c>

</xml_diff>